<commit_message>
Code to write cell data in excel
</commit_message>
<xml_diff>
--- a/Sanjay/src/main/java/Workbooks/Master.xlsx
+++ b/Sanjay/src/main/java/Workbooks/Master.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -44,6 +44,51 @@
   </si>
   <si>
     <t>String to be passed3</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Override</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>FieldListOne</t>
+  </si>
+  <si>
+    <t>OverrideListOne</t>
+  </si>
+  <si>
+    <t>StatusListOne</t>
+  </si>
+  <si>
+    <t>FieldListTwo</t>
+  </si>
+  <si>
+    <t>OverrideListTwo</t>
+  </si>
+  <si>
+    <t>StatusListTwo</t>
+  </si>
+  <si>
+    <t>FieldListThree</t>
+  </si>
+  <si>
+    <t>OverrideistThree</t>
+  </si>
+  <si>
+    <t>StatusListThree</t>
   </si>
 </sst>
 </file>
@@ -169,7 +214,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -177,13 +222,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>